<commit_message>
versão colocando postes ok
</commit_message>
<xml_diff>
--- a/TABELA ABACOS.xlsx
+++ b/TABELA ABACOS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESTE_PLOTAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\matriz_csv_to_kml\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
   <si>
     <t>tipo_poste</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>[(-1.0, 0.0), (-1.0, 217.143), (160.0, 217.143), (160.0, 0.0), (-1.0, 0.0)]]</t>
+  </si>
+  <si>
+    <t>rotacao_poste</t>
+  </si>
+  <si>
+    <t>topo1</t>
+  </si>
+  <si>
+    <t>bissetriz2</t>
   </si>
 </sst>
 </file>
@@ -913,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +943,7 @@
     <col min="11" max="11" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -966,10 +975,13 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -977,18 +989,27 @@
         <v>9</v>
       </c>
       <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -996,12 +1017,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1011,8 +1032,11 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1023,7 +1047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1034,7 +1058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1054,7 +1078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1065,7 +1089,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1082,7 +1106,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1093,7 +1117,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1101,7 +1125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1109,12 +1133,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>

</xml_diff>